<commit_message>
app is stable - pulling from excel and adding to page
</commit_message>
<xml_diff>
--- a/public/pa-promo-comparison-spreadsheet.xlsx
+++ b/public/pa-promo-comparison-spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://primaryarms-my.sharepoint.com/personal/oyoung_primaryarms_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{B2F9A66B-9732-42FB-ABF8-0440A18BF175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09FFC77-BA68-4DD0-9E0D-9CBEC4198D94}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{B2F9A66B-9732-42FB-ABF8-0440A18BF175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB720EE3-62AD-4BC1-8056-A98882DD8BC3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1875" windowWidth="20730" windowHeight="11040" xr2:uid="{49D8BD67-E44B-4EB8-8234-BD93867359F0}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{49D8BD67-E44B-4EB8-8234-BD93867359F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,34 +36,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Email Links</t>
+    <t>https://cors-anywhere.herokuapp.com/https://news.primaryarms.com/q/R2wAIrCyKnByoGxG1BC9dPcdY_eYGio1HHvBFO66scis4S-QZq4QmAXD2</t>
   </si>
   <si>
-    <t>https://cors-anywhere.herokuapp.com/https://news.primaryarms.com/q/R2wAIrCyKnByoGxG1BC9dPcdY_eYGio1HHvBFO66scis4S-QZq4QmAXD2</t>
+    <t>https://cors-anywhere.herokuapp.com/https://www.opticsplanet.com/view/email/791098eaeb6c3a8981d1917c1dbc3bb0</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -82,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -90,37 +87,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -456,35 +431,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9514E938-FDC4-499A-B43D-3F6E6AA7750C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="106.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>45369</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{22097B0C-CA16-4EAB-9497-5559687162D1}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{A1A62761-068D-49C1-9536-3965DCCD45C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>